<commit_message>
app is pretty developed
</commit_message>
<xml_diff>
--- a/directory_app/raw_data/WLAX_LETTERWINNER_DATA_complete.xlsx
+++ b/directory_app/raw_data/WLAX_LETTERWINNER_DATA_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracerotondo/Desktop/GOV1005 /Project/WLAX_Directory/directory_app/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6DFF92-9399-B24E-9A10-287804AED3A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD19184-48ED-4145-A2DC-FEF9F9AB7DBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="460" windowWidth="24780" windowHeight="16120" xr2:uid="{EA26E0FC-545C-F54D-9B10-F7662692507E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="1818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="1819">
   <si>
     <t>Name</t>
   </si>
@@ -5487,6 +5487,9 @@
   </si>
   <si>
     <t>Pforzheimer</t>
+  </si>
+  <si>
+    <t>Canning</t>
   </si>
 </sst>
 </file>
@@ -5910,14 +5913,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8520AADE-8F57-7342-A682-D1D49773B414}">
   <dimension ref="A1:Z364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="135" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L115" sqref="L115"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="135" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="27.1640625" customWidth="1"/>
@@ -12986,8 +12989,8 @@
     </row>
     <row r="152" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>Elizabeth Hansen</v>
+        <f>CONCATENATE(B152, " ", D152)</f>
+        <v>Elizabeth Canning</v>
       </c>
       <c r="B152" t="s">
         <v>51</v>
@@ -12996,7 +12999,7 @@
         <v>349</v>
       </c>
       <c r="D152" t="s">
-        <v>349</v>
+        <v>1818</v>
       </c>
       <c r="E152">
         <v>1992</v>

</xml_diff>